<commit_message>
Gacha api 로직 작성
다음 할일 - 쿠키
미래 목표 - 킹덤, 쿠키, 스테이지, 실시간 컨텐츠1개만 간단히 구축 (클라 포함)
</commit_message>
<xml_diff>
--- a/Data/Excel/Proto/Schedule.xlsx
+++ b/Data/Excel/Proto/Schedule.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitWorks\GameServerStudyAspNet\Data\Excel\Proto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3CB10CD-01D7-4D41-B8EE-F6205CC3EF7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F39EB15-2A6E-4E84-8D4B-045984C394BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B69D90B2-837F-4F1C-A343-AB9C9731F0BF}"/>
+    <workbookView xWindow="3510" yWindow="3510" windowWidth="22980" windowHeight="11295" xr2:uid="{B69D90B2-837F-4F1C-A343-AB9C9731F0BF}"/>
   </bookViews>
   <sheets>
     <sheet name="Ticket" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="12">
   <si>
     <t>Num</t>
     <phoneticPr fontId="18" type="noConversion"/>
@@ -1015,10 +1015,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEEB70FA-D65F-432A-8185-F0281658762C}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -1078,7 +1078,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>1000001</v>
+        <v>1001001</v>
       </c>
       <c r="B4" t="s">
         <v>4</v>
@@ -1093,6 +1093,46 @@
         <v>45736.999988425923</v>
       </c>
       <c r="F4" s="1">
+        <v>45736.999988425923</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>1002001</v>
+      </c>
+      <c r="B5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="1">
+        <v>45658</v>
+      </c>
+      <c r="D5" s="1">
+        <v>45658</v>
+      </c>
+      <c r="E5" s="1">
+        <v>45736.999988425923</v>
+      </c>
+      <c r="F5" s="1">
+        <v>45736.999988425923</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>1002002</v>
+      </c>
+      <c r="B6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="1">
+        <v>45658</v>
+      </c>
+      <c r="D6" s="1">
+        <v>45658</v>
+      </c>
+      <c r="E6" s="1">
+        <v>45736.999988425923</v>
+      </c>
+      <c r="F6" s="1">
         <v>45736.999988425923</v>
       </c>
     </row>

</xml_diff>